<commit_message>
Updates Standalone and WebChat
</commit_message>
<xml_diff>
--- a/doc/EventList.xlsx
+++ b/doc/EventList.xlsx
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changes GUI to Bootstrap per default && more
Adds a ProgressIndicator to the Standalone version
Adds new Events
Adds new Build-Style (compile)
   Only compiles. Used for Spell check and Lint
</commit_message>
<xml_diff>
--- a/doc/EventList.xlsx
+++ b/doc/EventList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
   <si>
     <t>Name</t>
   </si>
@@ -302,6 +302,132 @@
   </si>
   <si>
     <t>Result</t>
+  </si>
+  <si>
+    <t>standaloneInit</t>
+  </si>
+  <si>
+    <t>standaloneClearPage</t>
+  </si>
+  <si>
+    <t>Standalone - Initialize</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered before the page is cleared</t>
+  </si>
+  <si>
+    <t>standalonePreUpdatePage</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered before the page is updated</t>
+  </si>
+  <si>
+    <t>standalonePostUpdatePage</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered after the page is updated</t>
+  </si>
+  <si>
+    <t>standaloneOnHashTimerCreate</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when the Hash-Timer is created</t>
+  </si>
+  <si>
+    <t>standaloneOnHashTimerTick</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered on every Tick of the Hash-Timer</t>
+  </si>
+  <si>
+    <t>standaloneRunScript</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when the Script is loaded</t>
+  </si>
+  <si>
+    <t>standaloneOnStyleInsert</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when the PageStyle is inserted</t>
+  </si>
+  <si>
+    <t>PageStyle</t>
+  </si>
+  <si>
+    <t>standalonePreRequest</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered before a Request is made</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>standaloneOnRequestDone</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when a Request is done</t>
+  </si>
+  <si>
+    <t>{url, content}</t>
+  </si>
+  <si>
+    <t>standalonePreRequestCategories</t>
+  </si>
+  <si>
+    <t>standalonePostCategoriesRequest</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered before Categories are requested</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered after the Categories are loaded</t>
+  </si>
+  <si>
+    <t>CategoriesContent</t>
+  </si>
+  <si>
+    <t>standaloneCategoriesParsed</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when the Categories are parsed</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>standalonePreRequestElements</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered before Elements are requested</t>
+  </si>
+  <si>
+    <t>standalonePostRequestElements</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered after the Elements are loaded</t>
+  </si>
+  <si>
+    <t>ElementsContent</t>
+  </si>
+  <si>
+    <t>standaloneElementsParsed</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when the Elements are parsed</t>
+  </si>
+  <si>
+    <t>[Name, Elements]</t>
+  </si>
+  <si>
+    <t>standaloneOnRequestFail</t>
+  </si>
+  <si>
+    <t>Standalone - Is triggered when a Request fails</t>
+  </si>
+  <si>
+    <t>{url, event}</t>
   </si>
 </sst>
 </file>
@@ -663,15 +789,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D42"/>
+  <dimension ref="B3:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="61.5703125" customWidth="1"/>
     <col min="4" max="4" width="44.140625" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -1110,6 +1236,193 @@
         <v>95</v>
       </c>
     </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" t="s">
+        <v>121</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>129</v>
+      </c>
+      <c r="C58" t="s">
+        <v>130</v>
+      </c>
+      <c r="D58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>